<commit_message>
demo frieght rates 2
Former-commit-id: a9ba621d8e55a41359235a50e8120eef9cfb3515
</commit_message>
<xml_diff>
--- a/db/dummydata/demo/demo__freight_rates.xlsx
+++ b/db/dummydata/demo/demo__freight_rates.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="50">
   <si>
     <t>CUSTOMER_ID</t>
   </si>
@@ -13872,11 +13872,245 @@
         <v>1500.0</v>
       </c>
     </row>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="262" ht="12.75" customHeight="1">
+      <c r="D262" t="s">
+        <v>21</v>
+      </c>
+      <c r="E262" t="s">
+        <v>32</v>
+      </c>
+      <c r="F262" s="3">
+        <v>43174.0</v>
+      </c>
+      <c r="G262" s="3">
+        <v>43539.0</v>
+      </c>
+      <c r="H262" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I262" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J262" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="K262">
+        <v>1000.0</v>
+      </c>
+      <c r="L262" t="s">
+        <v>25</v>
+      </c>
+      <c r="M262" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N262" t="s">
+        <v>27</v>
+      </c>
+      <c r="O262" t="s">
+        <v>33</v>
+      </c>
+      <c r="P262">
+        <v>39.0</v>
+      </c>
+      <c r="Q262">
+        <v>39.0</v>
+      </c>
+      <c r="T262" s="4"/>
+    </row>
+    <row r="263" ht="12.75" customHeight="1">
+      <c r="D263" t="s">
+        <v>21</v>
+      </c>
+      <c r="E263" t="s">
+        <v>32</v>
+      </c>
+      <c r="F263" s="3">
+        <v>43174.0</v>
+      </c>
+      <c r="G263" s="3">
+        <v>43540.0</v>
+      </c>
+      <c r="H263" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I263" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J263" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="K263">
+        <v>1000.0</v>
+      </c>
+      <c r="L263" t="s">
+        <v>25</v>
+      </c>
+      <c r="M263" t="s">
+        <v>34</v>
+      </c>
+      <c r="N263" t="s">
+        <v>27</v>
+      </c>
+      <c r="O263" t="s">
+        <v>33</v>
+      </c>
+      <c r="P263">
+        <v>10.0</v>
+      </c>
+      <c r="Q263">
+        <v>4.0</v>
+      </c>
+      <c r="R263">
+        <v>550.0</v>
+      </c>
+      <c r="S263" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="264" ht="12.75" customHeight="1">
+      <c r="D264" t="s">
+        <v>21</v>
+      </c>
+      <c r="E264" t="s">
+        <v>32</v>
+      </c>
+      <c r="F264" s="3">
+        <v>43174.0</v>
+      </c>
+      <c r="G264" s="3">
+        <v>43541.0</v>
+      </c>
+      <c r="H264" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I264" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J264" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="K264">
+        <v>1000.0</v>
+      </c>
+      <c r="L264" t="s">
+        <v>25</v>
+      </c>
+      <c r="M264" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N264" t="s">
+        <v>27</v>
+      </c>
+      <c r="O264" t="s">
+        <v>33</v>
+      </c>
+      <c r="P264">
+        <v>0.0</v>
+      </c>
+      <c r="Q264">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="265" ht="12.75" customHeight="1">
+      <c r="D265" t="s">
+        <v>21</v>
+      </c>
+      <c r="E265" t="s">
+        <v>32</v>
+      </c>
+      <c r="F265" s="3">
+        <v>43174.0</v>
+      </c>
+      <c r="G265" s="3">
+        <v>43542.0</v>
+      </c>
+      <c r="H265" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I265" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J265" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="K265">
+        <v>1000.0</v>
+      </c>
+      <c r="L265" t="s">
+        <v>25</v>
+      </c>
+      <c r="M265" t="s">
+        <v>34</v>
+      </c>
+      <c r="N265" t="s">
+        <v>27</v>
+      </c>
+      <c r="O265" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q265">
+        <v>100.0</v>
+      </c>
+      <c r="S265" t="s">
+        <v>36</v>
+      </c>
+      <c r="T265">
+        <v>1500.0</v>
+      </c>
+      <c r="U265">
+        <v>2000.0</v>
+      </c>
+    </row>
+    <row r="266" ht="12.75" customHeight="1">
+      <c r="D266" t="s">
+        <v>21</v>
+      </c>
+      <c r="E266" t="s">
+        <v>32</v>
+      </c>
+      <c r="F266" s="3">
+        <v>43174.0</v>
+      </c>
+      <c r="G266" s="3">
+        <v>43543.0</v>
+      </c>
+      <c r="H266" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I266" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J266" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="K266">
+        <v>1000.0</v>
+      </c>
+      <c r="L266" t="s">
+        <v>25</v>
+      </c>
+      <c r="M266" t="s">
+        <v>34</v>
+      </c>
+      <c r="N266" t="s">
+        <v>27</v>
+      </c>
+      <c r="O266" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q266">
+        <v>250.0</v>
+      </c>
+      <c r="S266" t="s">
+        <v>36</v>
+      </c>
+      <c r="T266">
+        <v>2000.0</v>
+      </c>
+      <c r="U266">
+        <v>2500.0</v>
+      </c>
+    </row>
     <row r="267" ht="15.75" customHeight="1"/>
     <row r="268" ht="15.75" customHeight="1"/>
     <row r="269" ht="15.75" customHeight="1"/>

</xml_diff>